<commit_message>
Subida de archivos correspondientes a el trabajo teórico
</commit_message>
<xml_diff>
--- a/Obtención de casos de prueba.xlsx
+++ b/Obtención de casos de prueba.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orteg\Desktop\Uni\Año 3\1er Cuatrimestre\Ingenieria del Software II\Trabajo Teórico 2 Ejercicio 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\3º Ingeniería Informática\INGENIERÍA DEL SOFTWARE II\Trabajos\Ejercicio 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEB4C92-E833-45B5-B2A0-C36F6CF7196C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3394414-8A8B-44AB-848D-B7E0DB17F0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Apartado 7" sheetId="1" r:id="rId1"/>
+    <sheet name="Apartado 8" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="37">
   <si>
     <t>PARÁMETROS ENTRADA</t>
   </si>
@@ -143,6 +144,21 @@
   </si>
   <si>
     <t>TRAS COMBINACIÓN</t>
+  </si>
+  <si>
+    <t>Condición Dominante</t>
+  </si>
+  <si>
+    <t>A, B, C</t>
+  </si>
+  <si>
+    <t>A, B</t>
+  </si>
+  <si>
+    <t>A, C</t>
+  </si>
+  <si>
+    <t>B, C</t>
   </si>
 </sst>
 </file>
@@ -210,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -244,11 +260,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -267,6 +309,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -585,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1728,4 +1779,1283 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4720DC20-FE36-49D6-BA17-54C775E575C8}">
+  <dimension ref="A1:T59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2">
+        <v>17</v>
+      </c>
+      <c r="K2" s="2">
+        <v>26</v>
+      </c>
+      <c r="L2" s="2">
+        <v>18</v>
+      </c>
+      <c r="M2" s="2">
+        <v>17</v>
+      </c>
+      <c r="N2" s="2">
+        <v>19</v>
+      </c>
+      <c r="O2" s="2">
+        <v>17</v>
+      </c>
+      <c r="P2" s="2">
+        <v>19</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>24</v>
+      </c>
+      <c r="R2" s="2">
+        <v>25</v>
+      </c>
+      <c r="S2" s="2">
+        <v>24</v>
+      </c>
+      <c r="T2" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
+        <v>0</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>1</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="2">
+        <v>20</v>
+      </c>
+      <c r="J9" s="2">
+        <v>17</v>
+      </c>
+      <c r="K9" s="2">
+        <v>26</v>
+      </c>
+      <c r="L9" s="2">
+        <v>18</v>
+      </c>
+      <c r="M9" s="2">
+        <v>17</v>
+      </c>
+      <c r="N9" s="2">
+        <v>19</v>
+      </c>
+      <c r="O9" s="2">
+        <v>19</v>
+      </c>
+      <c r="P9" s="2">
+        <v>24</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>25</v>
+      </c>
+      <c r="R9" s="2">
+        <v>24</v>
+      </c>
+      <c r="S9" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>0</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
+        <v>0</v>
+      </c>
+      <c r="B13" s="9">
+        <v>0</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>1</v>
+      </c>
+      <c r="B18" s="8">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8">
+        <v>0</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>1</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>0</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>0</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="8">
+        <v>0</v>
+      </c>
+      <c r="B24" s="8">
+        <v>1</v>
+      </c>
+      <c r="C24" s="8">
+        <v>0</v>
+      </c>
+      <c r="D24" s="8">
+        <v>0</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
+        <v>0</v>
+      </c>
+      <c r="B25" s="6">
+        <v>1</v>
+      </c>
+      <c r="C25" s="6">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
+        <v>1</v>
+      </c>
+      <c r="B26" s="6">
+        <v>0</v>
+      </c>
+      <c r="C26" s="6">
+        <v>0</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="9">
+        <v>1</v>
+      </c>
+      <c r="B27" s="9">
+        <v>0</v>
+      </c>
+      <c r="C27" s="9">
+        <v>1</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>0</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
+        <v>0</v>
+      </c>
+      <c r="B33" s="8">
+        <v>0</v>
+      </c>
+      <c r="C33" s="8">
+        <v>1</v>
+      </c>
+      <c r="D33" s="8">
+        <v>0</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="6">
+        <v>0</v>
+      </c>
+      <c r="B34" s="6">
+        <v>1</v>
+      </c>
+      <c r="C34" s="6">
+        <v>0</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="9">
+        <v>0</v>
+      </c>
+      <c r="B35" s="9">
+        <v>1</v>
+      </c>
+      <c r="C35" s="9">
+        <v>1</v>
+      </c>
+      <c r="D35" s="9">
+        <v>0</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="8">
+        <v>1</v>
+      </c>
+      <c r="B36" s="8">
+        <v>0</v>
+      </c>
+      <c r="C36" s="8">
+        <v>0</v>
+      </c>
+      <c r="D36" s="8">
+        <v>0</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="6">
+        <v>1</v>
+      </c>
+      <c r="B37" s="6">
+        <v>0</v>
+      </c>
+      <c r="C37" s="6">
+        <v>1</v>
+      </c>
+      <c r="D37" s="6">
+        <v>1</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="9">
+        <v>1</v>
+      </c>
+      <c r="B38" s="9">
+        <v>1</v>
+      </c>
+      <c r="C38" s="9">
+        <v>0</v>
+      </c>
+      <c r="D38" s="9">
+        <v>0</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>1</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>0</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>0</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="8">
+        <v>0</v>
+      </c>
+      <c r="B44" s="8">
+        <v>1</v>
+      </c>
+      <c r="C44" s="8">
+        <v>0</v>
+      </c>
+      <c r="D44" s="8">
+        <v>0</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="6">
+        <v>0</v>
+      </c>
+      <c r="B45" s="6">
+        <v>1</v>
+      </c>
+      <c r="C45" s="6">
+        <v>1</v>
+      </c>
+      <c r="D45" s="6">
+        <v>0</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="6">
+        <v>1</v>
+      </c>
+      <c r="B46" s="6">
+        <v>0</v>
+      </c>
+      <c r="C46" s="6">
+        <v>0</v>
+      </c>
+      <c r="D46" s="6">
+        <v>1</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="9">
+        <v>1</v>
+      </c>
+      <c r="B47" s="9">
+        <v>0</v>
+      </c>
+      <c r="C47" s="9">
+        <v>1</v>
+      </c>
+      <c r="D47" s="9">
+        <v>0</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>1</v>
+      </c>
+      <c r="B48" s="2">
+        <v>1</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>1</v>
+      </c>
+      <c r="B49" s="2">
+        <v>1</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>0</v>
+      </c>
+      <c r="B52" s="2">
+        <v>0</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="8">
+        <v>0</v>
+      </c>
+      <c r="B53" s="8">
+        <v>0</v>
+      </c>
+      <c r="C53" s="8">
+        <v>1</v>
+      </c>
+      <c r="D53" s="8">
+        <v>0</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="6">
+        <v>0</v>
+      </c>
+      <c r="B54" s="6">
+        <v>1</v>
+      </c>
+      <c r="C54" s="6">
+        <v>0</v>
+      </c>
+      <c r="D54" s="6">
+        <v>0</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="9">
+        <v>0</v>
+      </c>
+      <c r="B55" s="9">
+        <v>1</v>
+      </c>
+      <c r="C55" s="9">
+        <v>1</v>
+      </c>
+      <c r="D55" s="9">
+        <v>0</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="8">
+        <v>1</v>
+      </c>
+      <c r="B56" s="8">
+        <v>0</v>
+      </c>
+      <c r="C56" s="8">
+        <v>0</v>
+      </c>
+      <c r="D56" s="8">
+        <v>0</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="6">
+        <v>1</v>
+      </c>
+      <c r="B57" s="6">
+        <v>0</v>
+      </c>
+      <c r="C57" s="6">
+        <v>1</v>
+      </c>
+      <c r="D57" s="6">
+        <v>1</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="9">
+        <v>1</v>
+      </c>
+      <c r="B58" s="9">
+        <v>1</v>
+      </c>
+      <c r="C58" s="9">
+        <v>0</v>
+      </c>
+      <c r="D58" s="9">
+        <v>0</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>1</v>
+      </c>
+      <c r="B59" s="2">
+        <v>1</v>
+      </c>
+      <c r="C59" s="2">
+        <v>1</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>